<commit_message>
rebased on AU Core and updated narrative
</commit_message>
<xml_diff>
--- a/StructureDefinition-ARFAllergy.xlsx
+++ b/StructureDefinition-ARFAllergy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-21T11:55:01+10:00</t>
+    <t>2024-05-21T16:48:43+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://hl7.org.au/fhir/StructureDefinition/au-allergyintolerance</t>
+    <t>http://hl7.org.au/fhir/core/StructureDefinition/au-core-allergyintolerance</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -706,7 +706,7 @@
     <t>AllergyIntolerance.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-encounter)
 </t>
   </si>
   <si>
@@ -726,7 +726,7 @@
   </si>
   <si>
     <t>dateTime
-AgePeriodRangestring</t>
+AgePeriodRange</t>
   </si>
   <si>
     <t>When allergy or intolerance was identified</t>
@@ -770,7 +770,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|http://hl7.org.au/fhir/core/StructureDefinition/au-core-relatedperson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
 </t>
   </si>
   <si>
@@ -793,7 +793,7 @@
 Informant</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient|RelatedPerson|Practitioner|PractitionerRole)
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|http://hl7.org.au/fhir/core/StructureDefinition/au-core-relatedperson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
 </t>
   </si>
   <si>
@@ -1363,7 +1363,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="70.4296875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2865,7 +2865,7 @@
         <v>86</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s" s="2">
         <v>78</v>
@@ -3307,7 +3307,7 @@
         <v>86</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s" s="2">
         <v>78</v>
@@ -3416,7 +3416,7 @@
         <v>86</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>78</v>
@@ -3525,7 +3525,7 @@
         <v>86</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>78</v>
@@ -3743,7 +3743,7 @@
         <v>86</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>78</v>
@@ -3852,7 +3852,7 @@
         <v>86</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>78</v>
@@ -4074,7 +4074,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>78</v>
@@ -4185,7 +4185,7 @@
         <v>77</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>78</v>
@@ -4627,7 +4627,7 @@
         <v>86</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>78</v>
@@ -4736,7 +4736,7 @@
         <v>77</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>78</v>
@@ -5065,7 +5065,7 @@
         <v>86</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>78</v>

</xml_diff>

<commit_message>
updates to narrative and examples
</commit_message>
<xml_diff>
--- a/StructureDefinition-ARFAllergy.xlsx
+++ b/StructureDefinition-ARFAllergy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-21T16:48:43+10:00</t>
+    <t>2024-05-23T13:27:21+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -770,7 +770,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|http://hl7.org.au/fhir/core/StructureDefinition/au-core-relatedperson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|RelatedPerson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
 </t>
   </si>
   <si>
@@ -793,7 +793,7 @@
 Informant</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|http://hl7.org.au/fhir/core/StructureDefinition/au-core-relatedperson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|RelatedPerson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
 </t>
   </si>
   <si>
@@ -1363,7 +1363,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="209.48828125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2865,7 +2865,7 @@
         <v>86</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s" s="2">
         <v>78</v>
@@ -4627,7 +4627,7 @@
         <v>86</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>78</v>

</xml_diff>

<commit_message>
Updates from new publisher and sushi versions.  Added README
</commit_message>
<xml_diff>
--- a/StructureDefinition-ARFAllergy.xlsx
+++ b/StructureDefinition-ARFAllergy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="320">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.3</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-30T15:43:42+10:00</t>
+    <t>2024-10-24T17:10:08+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -653,6 +653,9 @@
 When a substance or product code is specified for the 'code' element, the "default" semantic context is that this is a positive statement of an allergy or intolerance (depending on the value of the 'type' element, if present) condition to the specified substance/product.  In the corresponding SNOMED CT allergy model, the specified substance/product is the target (destination) of the "Causative agent" relationship.  The 'substanceExposureRisk' extension is available as a structured and more flexible alternative to the 'code' element for making positive or negative allergy or intolerance statements.  This extension provides the capability to make "no known allergy" (or "no risk of adverse reaction") statements regarding any coded substance/product (including cases when a pre-coordinated "no allergy to x" concept for that substance/product does not exist).  If the 'substanceExposureRisk' extension is present, the AllergyIntolerance.code element SHALL be omitted.</t>
+  </si>
+  <si>
+    <t>extensible</t>
   </si>
   <si>
     <t>https://healthterminologies.gov.au/fhir/ValueSet/indicator-hypersensitivity-intolerance-to-substance-2</t>
@@ -706,7 +709,7 @@
     <t>AllergyIntolerance.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-encounter)
+    <t xml:space="preserve">Reference(Encounter)
 </t>
   </si>
   <si>
@@ -770,7 +773,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|RelatedPerson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
+    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Patient|RelatedPerson)
 </t>
   </si>
   <si>
@@ -793,7 +796,7 @@
 Informant</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/core/StructureDefinition/au-core-patient|RelatedPerson|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitioner|http://hl7.org.au/fhir/core/StructureDefinition/au-core-practitionerrole)
+    <t xml:space="preserve">Reference(Patient|RelatedPerson|Practitioner|PractitionerRole)
 </t>
   </si>
   <si>
@@ -1363,7 +1366,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="209.48828125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="70.4296875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -3242,11 +3245,11 @@
         <v>78</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>78</v>
@@ -3279,25 +3282,25 @@
         <v>98</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
@@ -3316,13 +3319,13 @@
         <v>87</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3373,7 +3376,7 @@
         <v>78</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>86</v>
@@ -3388,21 +3391,21 @@
         <v>98</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3416,7 +3419,7 @@
         <v>86</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>78</v>
@@ -3425,13 +3428,13 @@
         <v>78</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -3482,7 +3485,7 @@
         <v>78</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>76</v>
@@ -3497,10 +3500,10 @@
         <v>98</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>78</v>
@@ -3508,10 +3511,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3534,13 +3537,13 @@
         <v>78</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3591,7 +3594,7 @@
         <v>78</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>76</v>
@@ -3606,10 +3609,10 @@
         <v>98</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>78</v>
@@ -3617,10 +3620,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3643,13 +3646,13 @@
         <v>78</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -3700,7 +3703,7 @@
         <v>78</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>76</v>
@@ -3715,25 +3718,25 @@
         <v>98</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
@@ -3743,7 +3746,7 @@
         <v>86</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>78</v>
@@ -3752,13 +3755,13 @@
         <v>78</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3809,7 +3812,7 @@
         <v>78</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>76</v>
@@ -3824,10 +3827,10 @@
         <v>98</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>78</v>
@@ -3835,14 +3838,14 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -3852,7 +3855,7 @@
         <v>86</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>78</v>
@@ -3861,16 +3864,16 @@
         <v>87</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -3920,7 +3923,7 @@
         <v>78</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>76</v>
@@ -3935,21 +3938,21 @@
         <v>98</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3972,16 +3975,16 @@
         <v>78</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4031,7 +4034,7 @@
         <v>78</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>76</v>
@@ -4046,7 +4049,7 @@
         <v>98</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>78</v>
@@ -4057,10 +4060,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4074,7 +4077,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>78</v>
@@ -4083,16 +4086,16 @@
         <v>78</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -4142,7 +4145,7 @@
         <v>78</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>76</v>
@@ -4157,7 +4160,7 @@
         <v>98</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>78</v>
@@ -4168,10 +4171,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4194,13 +4197,13 @@
         <v>78</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -4251,7 +4254,7 @@
         <v>78</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>76</v>
@@ -4266,7 +4269,7 @@
         <v>98</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>78</v>
@@ -4277,10 +4280,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4303,13 +4306,13 @@
         <v>78</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4360,7 +4363,7 @@
         <v>78</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>76</v>
@@ -4375,7 +4378,7 @@
         <v>78</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>78</v>
@@ -4386,10 +4389,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4418,7 +4421,7 @@
         <v>133</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="N28" t="s" s="2">
         <v>135</v>
@@ -4471,7 +4474,7 @@
         <v>78</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>76</v>
@@ -4486,7 +4489,7 @@
         <v>137</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>78</v>
@@ -4497,14 +4500,14 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -4526,10 +4529,10 @@
         <v>132</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="N29" t="s" s="2">
         <v>135</v>
@@ -4584,7 +4587,7 @@
         <v>78</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>76</v>
@@ -4610,10 +4613,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4639,13 +4642,13 @@
         <v>153</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -4675,7 +4678,7 @@
       </c>
       <c r="Y30" s="2"/>
       <c r="Z30" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>78</v>
@@ -4693,7 +4696,7 @@
         <v>78</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>76</v>
@@ -4708,7 +4711,7 @@
         <v>98</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>78</v>
@@ -4719,14 +4722,14 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -4748,13 +4751,13 @@
         <v>153</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -4784,7 +4787,7 @@
       </c>
       <c r="Y31" s="2"/>
       <c r="Z31" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>78</v>
@@ -4802,7 +4805,7 @@
         <v>78</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>86</v>
@@ -4823,19 +4826,19 @@
         <v>78</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -4854,16 +4857,16 @@
         <v>78</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -4913,7 +4916,7 @@
         <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>76</v>
@@ -4928,7 +4931,7 @@
         <v>98</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>78</v>
@@ -4939,10 +4942,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -4965,13 +4968,13 @@
         <v>78</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5022,7 +5025,7 @@
         <v>78</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>76</v>
@@ -5037,21 +5040,21 @@
         <v>98</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5077,13 +5080,13 @@
         <v>106</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -5112,10 +5115,10 @@
         <v>157</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="Z34" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AA34" t="s" s="2">
         <v>78</v>
@@ -5133,7 +5136,7 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>76</v>
@@ -5159,10 +5162,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5188,13 +5191,13 @@
         <v>153</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5224,7 +5227,7 @@
       </c>
       <c r="Y35" s="2"/>
       <c r="Z35" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>78</v>
@@ -5242,7 +5245,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>76</v>
@@ -5257,7 +5260,7 @@
         <v>98</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>78</v>
@@ -5268,10 +5271,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5294,16 +5297,16 @@
         <v>78</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -5353,7 +5356,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>76</v>
@@ -5368,7 +5371,7 @@
         <v>98</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>78</v>

</xml_diff>